<commit_message>
i think not in use anymore
</commit_message>
<xml_diff>
--- a/clp/results/_comparison_plots/merged_BR_original_summaries.xlsx
+++ b/clp/results/_comparison_plots/merged_BR_original_summaries.xlsx
@@ -751,7 +751,7 @@
       </c>
       <c r="AM2" t="inlineStr">
         <is>
-          <t>Baseline-DBLF</t>
+          <t>DBLF</t>
         </is>
       </c>
     </row>
@@ -876,7 +876,7 @@
       </c>
       <c r="AM3" t="inlineStr">
         <is>
-          <t>Baseline-DBLF</t>
+          <t>DBLF</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="AM4" t="inlineStr">
         <is>
-          <t>Baseline-DBLF</t>
+          <t>DBLF</t>
         </is>
       </c>
     </row>
@@ -1126,7 +1126,7 @@
       </c>
       <c r="AM5" t="inlineStr">
         <is>
-          <t>Baseline-DBLF</t>
+          <t>DBLF</t>
         </is>
       </c>
     </row>
@@ -1251,7 +1251,7 @@
       </c>
       <c r="AM6" t="inlineStr">
         <is>
-          <t>Baseline-DBLF</t>
+          <t>DBLF</t>
         </is>
       </c>
     </row>
@@ -1376,7 +1376,7 @@
       </c>
       <c r="AM7" t="inlineStr">
         <is>
-          <t>Baseline-DBLF</t>
+          <t>DBLF</t>
         </is>
       </c>
     </row>
@@ -1501,7 +1501,7 @@
       </c>
       <c r="AM8" t="inlineStr">
         <is>
-          <t>Baseline-DBLF</t>
+          <t>DBLF</t>
         </is>
       </c>
     </row>
@@ -1626,7 +1626,7 @@
       </c>
       <c r="AM9" t="inlineStr">
         <is>
-          <t>Baseline-DBLF</t>
+          <t>DBLF</t>
         </is>
       </c>
     </row>
@@ -1751,7 +1751,7 @@
       </c>
       <c r="AM10" t="inlineStr">
         <is>
-          <t>Baseline-DBLF</t>
+          <t>DBLF</t>
         </is>
       </c>
     </row>
@@ -1876,7 +1876,7 @@
       </c>
       <c r="AM11" t="inlineStr">
         <is>
-          <t>Baseline-DBLF</t>
+          <t>DBLF</t>
         </is>
       </c>
     </row>
@@ -2001,7 +2001,7 @@
       </c>
       <c r="AM12" t="inlineStr">
         <is>
-          <t>Baseline-DBLF</t>
+          <t>DBLF</t>
         </is>
       </c>
     </row>
@@ -2126,7 +2126,7 @@
       </c>
       <c r="AM13" t="inlineStr">
         <is>
-          <t>Baseline-DBLF</t>
+          <t>DBLF</t>
         </is>
       </c>
     </row>
@@ -2251,7 +2251,7 @@
       </c>
       <c r="AM14" t="inlineStr">
         <is>
-          <t>Baseline-DBLF</t>
+          <t>DBLF</t>
         </is>
       </c>
     </row>
@@ -2376,7 +2376,7 @@
       </c>
       <c r="AM15" t="inlineStr">
         <is>
-          <t>Baseline-DBLF</t>
+          <t>DBLF</t>
         </is>
       </c>
     </row>
@@ -2501,7 +2501,7 @@
       </c>
       <c r="AM16" t="inlineStr">
         <is>
-          <t>Baseline-DBLF</t>
+          <t>DBLF</t>
         </is>
       </c>
     </row>
@@ -2626,7 +2626,7 @@
       </c>
       <c r="AM17" t="inlineStr">
         <is>
-          <t>Baseline-DBLF</t>
+          <t>DBLF</t>
         </is>
       </c>
     </row>
@@ -2751,7 +2751,7 @@
       </c>
       <c r="AM18" t="inlineStr">
         <is>
-          <t>Baseline-DBLF</t>
+          <t>DBLF</t>
         </is>
       </c>
     </row>
@@ -2876,7 +2876,7 @@
       </c>
       <c r="AM19" t="inlineStr">
         <is>
-          <t>Baseline-DBLF</t>
+          <t>DBLF</t>
         </is>
       </c>
     </row>
@@ -3001,7 +3001,7 @@
       </c>
       <c r="AM20" t="inlineStr">
         <is>
-          <t>Baseline-DBLF</t>
+          <t>DBLF</t>
         </is>
       </c>
     </row>
@@ -3126,7 +3126,7 @@
       </c>
       <c r="AM21" t="inlineStr">
         <is>
-          <t>Baseline-DBLF</t>
+          <t>DBLF</t>
         </is>
       </c>
     </row>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="AM22" t="inlineStr">
         <is>
-          <t>Baseline-DBLF</t>
+          <t>DBLF</t>
         </is>
       </c>
     </row>
@@ -3376,7 +3376,7 @@
       </c>
       <c r="AM23" t="inlineStr">
         <is>
-          <t>Baseline-DBLF</t>
+          <t>DBLF</t>
         </is>
       </c>
     </row>
@@ -3501,7 +3501,7 @@
       </c>
       <c r="AM24" t="inlineStr">
         <is>
-          <t>Baseline-DBLF</t>
+          <t>DBLF</t>
         </is>
       </c>
     </row>
@@ -3626,7 +3626,7 @@
       </c>
       <c r="AM25" t="inlineStr">
         <is>
-          <t>Baseline-DBLF</t>
+          <t>DBLF</t>
         </is>
       </c>
     </row>
@@ -3751,7 +3751,7 @@
       </c>
       <c r="AM26" t="inlineStr">
         <is>
-          <t>Baseline-DBLF</t>
+          <t>DBLF</t>
         </is>
       </c>
     </row>
@@ -3876,7 +3876,7 @@
       </c>
       <c r="AM27" t="inlineStr">
         <is>
-          <t>Baseline-DBLF</t>
+          <t>DBLF</t>
         </is>
       </c>
     </row>
@@ -4001,7 +4001,7 @@
       </c>
       <c r="AM28" t="inlineStr">
         <is>
-          <t>Baseline-DBLF</t>
+          <t>DBLF</t>
         </is>
       </c>
     </row>
@@ -4126,7 +4126,7 @@
       </c>
       <c r="AM29" t="inlineStr">
         <is>
-          <t>Baseline-DBLF</t>
+          <t>DBLF</t>
         </is>
       </c>
     </row>
@@ -4251,7 +4251,7 @@
       </c>
       <c r="AM30" t="inlineStr">
         <is>
-          <t>Baseline-DBLF</t>
+          <t>DBLF</t>
         </is>
       </c>
     </row>
@@ -4376,7 +4376,7 @@
       </c>
       <c r="AM31" t="inlineStr">
         <is>
-          <t>Baseline-DBLF</t>
+          <t>DBLF</t>
         </is>
       </c>
     </row>
@@ -4501,7 +4501,7 @@
       </c>
       <c r="AM32" t="inlineStr">
         <is>
-          <t>Baseline-DBLF</t>
+          <t>DBLF</t>
         </is>
       </c>
     </row>
@@ -4626,7 +4626,7 @@
       </c>
       <c r="AM33" t="inlineStr">
         <is>
-          <t>Baseline-DBLF</t>
+          <t>DBLF</t>
         </is>
       </c>
     </row>
@@ -4751,7 +4751,7 @@
       </c>
       <c r="AM34" t="inlineStr">
         <is>
-          <t>Two-Phase-DBLF</t>
+          <t>Ballance-Aware-DBLF</t>
         </is>
       </c>
     </row>
@@ -4876,7 +4876,7 @@
       </c>
       <c r="AM35" t="inlineStr">
         <is>
-          <t>Two-Phase-DBLF</t>
+          <t>Ballance-Aware-DBLF</t>
         </is>
       </c>
     </row>
@@ -5001,7 +5001,7 @@
       </c>
       <c r="AM36" t="inlineStr">
         <is>
-          <t>Two-Phase-DBLF</t>
+          <t>Ballance-Aware-DBLF</t>
         </is>
       </c>
     </row>
@@ -5126,7 +5126,7 @@
       </c>
       <c r="AM37" t="inlineStr">
         <is>
-          <t>Two-Phase-DBLF</t>
+          <t>Ballance-Aware-DBLF</t>
         </is>
       </c>
     </row>
@@ -5251,7 +5251,7 @@
       </c>
       <c r="AM38" t="inlineStr">
         <is>
-          <t>Two-Phase-DBLF</t>
+          <t>Ballance-Aware-DBLF</t>
         </is>
       </c>
     </row>
@@ -5376,7 +5376,7 @@
       </c>
       <c r="AM39" t="inlineStr">
         <is>
-          <t>Two-Phase-DBLF</t>
+          <t>Ballance-Aware-DBLF</t>
         </is>
       </c>
     </row>
@@ -5501,7 +5501,7 @@
       </c>
       <c r="AM40" t="inlineStr">
         <is>
-          <t>Two-Phase-DBLF</t>
+          <t>Ballance-Aware-DBLF</t>
         </is>
       </c>
     </row>
@@ -5626,7 +5626,7 @@
       </c>
       <c r="AM41" t="inlineStr">
         <is>
-          <t>Two-Phase-DBLF</t>
+          <t>Ballance-Aware-DBLF</t>
         </is>
       </c>
     </row>
@@ -5751,7 +5751,7 @@
       </c>
       <c r="AM42" t="inlineStr">
         <is>
-          <t>Two-Phase-DBLF</t>
+          <t>Ballance-Aware-DBLF</t>
         </is>
       </c>
     </row>
@@ -5876,7 +5876,7 @@
       </c>
       <c r="AM43" t="inlineStr">
         <is>
-          <t>Two-Phase-DBLF</t>
+          <t>Ballance-Aware-DBLF</t>
         </is>
       </c>
     </row>
@@ -6001,7 +6001,7 @@
       </c>
       <c r="AM44" t="inlineStr">
         <is>
-          <t>Two-Phase-DBLF</t>
+          <t>Ballance-Aware-DBLF</t>
         </is>
       </c>
     </row>
@@ -6126,7 +6126,7 @@
       </c>
       <c r="AM45" t="inlineStr">
         <is>
-          <t>Two-Phase-DBLF</t>
+          <t>Ballance-Aware-DBLF</t>
         </is>
       </c>
     </row>
@@ -6251,7 +6251,7 @@
       </c>
       <c r="AM46" t="inlineStr">
         <is>
-          <t>Two-Phase-DBLF</t>
+          <t>Ballance-Aware-DBLF</t>
         </is>
       </c>
     </row>
@@ -6376,7 +6376,7 @@
       </c>
       <c r="AM47" t="inlineStr">
         <is>
-          <t>Two-Phase-DBLF</t>
+          <t>Ballance-Aware-DBLF</t>
         </is>
       </c>
     </row>
@@ -6501,7 +6501,7 @@
       </c>
       <c r="AM48" t="inlineStr">
         <is>
-          <t>Two-Phase-DBLF</t>
+          <t>Ballance-Aware-DBLF</t>
         </is>
       </c>
     </row>
@@ -6626,7 +6626,7 @@
       </c>
       <c r="AM49" t="inlineStr">
         <is>
-          <t>Two-Phase-DBLF</t>
+          <t>Ballance-Aware-DBLF</t>
         </is>
       </c>
     </row>
@@ -6751,7 +6751,7 @@
       </c>
       <c r="AM50" t="inlineStr">
         <is>
-          <t>Two-Phase-DBLF</t>
+          <t>Ballance-Aware-DBLF</t>
         </is>
       </c>
     </row>
@@ -6876,7 +6876,7 @@
       </c>
       <c r="AM51" t="inlineStr">
         <is>
-          <t>Two-Phase-DBLF</t>
+          <t>Ballance-Aware-DBLF</t>
         </is>
       </c>
     </row>
@@ -7001,7 +7001,7 @@
       </c>
       <c r="AM52" t="inlineStr">
         <is>
-          <t>Two-Phase-DBLF</t>
+          <t>Ballance-Aware-DBLF</t>
         </is>
       </c>
     </row>
@@ -7126,7 +7126,7 @@
       </c>
       <c r="AM53" t="inlineStr">
         <is>
-          <t>Two-Phase-DBLF</t>
+          <t>Ballance-Aware-DBLF</t>
         </is>
       </c>
     </row>
@@ -7251,7 +7251,7 @@
       </c>
       <c r="AM54" t="inlineStr">
         <is>
-          <t>Two-Phase-DBLF</t>
+          <t>Ballance-Aware-DBLF</t>
         </is>
       </c>
     </row>
@@ -7376,7 +7376,7 @@
       </c>
       <c r="AM55" t="inlineStr">
         <is>
-          <t>Two-Phase-DBLF</t>
+          <t>Ballance-Aware-DBLF</t>
         </is>
       </c>
     </row>
@@ -7501,7 +7501,7 @@
       </c>
       <c r="AM56" t="inlineStr">
         <is>
-          <t>Two-Phase-DBLF</t>
+          <t>Ballance-Aware-DBLF</t>
         </is>
       </c>
     </row>
@@ -7626,7 +7626,7 @@
       </c>
       <c r="AM57" t="inlineStr">
         <is>
-          <t>Two-Phase-DBLF</t>
+          <t>Ballance-Aware-DBLF</t>
         </is>
       </c>
     </row>
@@ -7751,7 +7751,7 @@
       </c>
       <c r="AM58" t="inlineStr">
         <is>
-          <t>Two-Phase-DBLF</t>
+          <t>Ballance-Aware-DBLF</t>
         </is>
       </c>
     </row>
@@ -7876,7 +7876,7 @@
       </c>
       <c r="AM59" t="inlineStr">
         <is>
-          <t>Two-Phase-DBLF</t>
+          <t>Ballance-Aware-DBLF</t>
         </is>
       </c>
     </row>
@@ -8001,7 +8001,7 @@
       </c>
       <c r="AM60" t="inlineStr">
         <is>
-          <t>Two-Phase-DBLF</t>
+          <t>Ballance-Aware-DBLF</t>
         </is>
       </c>
     </row>
@@ -8126,7 +8126,7 @@
       </c>
       <c r="AM61" t="inlineStr">
         <is>
-          <t>Two-Phase-DBLF</t>
+          <t>Ballance-Aware-DBLF</t>
         </is>
       </c>
     </row>
@@ -8251,7 +8251,7 @@
       </c>
       <c r="AM62" t="inlineStr">
         <is>
-          <t>Two-Phase-DBLF</t>
+          <t>Ballance-Aware-DBLF</t>
         </is>
       </c>
     </row>
@@ -8376,7 +8376,7 @@
       </c>
       <c r="AM63" t="inlineStr">
         <is>
-          <t>Two-Phase-DBLF</t>
+          <t>Ballance-Aware-DBLF</t>
         </is>
       </c>
     </row>
@@ -8501,7 +8501,7 @@
       </c>
       <c r="AM64" t="inlineStr">
         <is>
-          <t>Two-Phase-DBLF</t>
+          <t>Ballance-Aware-DBLF</t>
         </is>
       </c>
     </row>
@@ -8626,7 +8626,7 @@
       </c>
       <c r="AM65" t="inlineStr">
         <is>
-          <t>Two-Phase-DBLF</t>
+          <t>Ballance-Aware-DBLF</t>
         </is>
       </c>
     </row>

</xml_diff>